<commit_message>
New Pay Bill scenario, Removal of run time parameters.
</commit_message>
<xml_diff>
--- a/TellerMate_FrameWork/TestData/testData.xlsx
+++ b/TellerMate_FrameWork/TestData/testData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Bills" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,12 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Cantt@mc.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Abc@1234</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Ref. No.</t>
+  </si>
+  <si>
+    <t>Bill ID</t>
+  </si>
+  <si>
+    <t>SNGPL</t>
+  </si>
+  <si>
+    <t>dha@mc.com</t>
+  </si>
+  <si>
+    <t>37522010000</t>
   </si>
 </sst>
 </file>
@@ -69,9 +85,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -355,9 +372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -367,10 +382,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -380,4 +395,41 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Explicit wait and other modifications.
</commit_message>
<xml_diff>
--- a/TellerMate_FrameWork/TestData/testData.xlsx
+++ b/TellerMate_FrameWork/TestData/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,10 @@
     <t>SNGPL</t>
   </si>
   <si>
-    <t>dha@mc.com</t>
-  </si>
-  <si>
-    <t>37522010000</t>
+    <t>99974010169</t>
+  </si>
+  <si>
+    <t>Cantt@mc.com</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -382,7 +382,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -401,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -426,7 +426,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>